<commit_message>
add tier Misc classic
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_BART_Demographics_20190630.xlsx
+++ b/inputs/data_raw/Data_BART_Demographics_20190630.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_BART\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA33B29B-5A8F-4D5D-91BF-64E5BF3560BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8466A9B9-4A04-48FC-9D8F-52B217A420A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1500" windowWidth="29040" windowHeight="15840" tabRatio="723" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="723" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="actives_misc" sheetId="19" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="127">
   <si>
     <t>TOC</t>
   </si>
@@ -1196,6 +1196,9 @@
   <si>
     <t>benefit</t>
   </si>
+  <si>
+    <t>sum</t>
+  </si>
 </sst>
 </file>
 
@@ -1205,7 +1208,7 @@
     <numFmt numFmtId="164" formatCode="\$#,##0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0;&quot;$&quot;\-#,##0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1312,6 +1315,14 @@
       <sz val="15.5"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1427,7 +1438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1728,6 +1739,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2501,8 +2513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB403699-3710-4596-97B0-B33CB2C2CC4F}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4796,10 +4808,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F61A781-B9B1-4F2B-BAEA-4245EA889B53}">
-  <dimension ref="A1:P42"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5754,44 +5766,408 @@
     </row>
     <row r="35" spans="6:16">
       <c r="F35" s="99"/>
+      <c r="G35">
+        <f>G7*G20</f>
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ref="H35:L35" si="0">H7*H20</f>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>20666</v>
+      </c>
       <c r="P35" s="15"/>
     </row>
     <row r="36" spans="6:16">
       <c r="F36" s="99"/>
+      <c r="G36">
+        <f t="shared" ref="G36:L50" si="1">G8*G21</f>
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>60594</v>
+      </c>
     </row>
     <row r="37" spans="6:16">
       <c r="F37" s="99"/>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>1972</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="1"/>
+        <v>178960</v>
+      </c>
     </row>
     <row r="38" spans="6:16">
       <c r="F38" s="99"/>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>2380</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="1"/>
+        <v>132440</v>
+      </c>
     </row>
     <row r="39" spans="6:16">
       <c r="F39" s="99"/>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>77700</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>2187</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>4974</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="1"/>
+        <v>201030</v>
+      </c>
     </row>
     <row r="40" spans="6:16">
       <c r="F40" s="99"/>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>912030</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>8814</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>1444</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>23071</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="1"/>
+        <v>308730</v>
+      </c>
     </row>
     <row r="41" spans="6:16">
       <c r="F41" s="99"/>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>4971806</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>130192</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>28400</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="1"/>
+        <v>292158</v>
+      </c>
     </row>
     <row r="42" spans="6:16">
       <c r="F42" s="99"/>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>16214269</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>255430</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>14700</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="1"/>
+        <v>128184</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="1"/>
+        <v>720615</v>
+      </c>
+    </row>
+    <row r="43" spans="6:16">
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>28421373</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>207647</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>1030</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>56202</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="1"/>
+        <v>1938699</v>
+      </c>
+    </row>
+    <row r="44" spans="6:16">
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>32265558</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="1"/>
+        <v>351158</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>22788</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="1"/>
+        <v>105660</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="1"/>
+        <v>797</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="1"/>
+        <v>3347934</v>
+      </c>
+    </row>
+    <row r="45" spans="6:16">
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>16671373</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="1"/>
+        <v>71508</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>2960</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>80066</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="1"/>
+        <v>2888152</v>
+      </c>
+    </row>
+    <row r="46" spans="6:16">
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>8177603</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>104392</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="1"/>
+        <v>27552</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="1"/>
+        <v>1401532</v>
+      </c>
+    </row>
+    <row r="47" spans="6:16">
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>4691156</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>38776</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>642</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="1"/>
+        <v>57072</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="1"/>
+        <v>1655933</v>
+      </c>
+    </row>
+    <row r="48" spans="6:16">
+      <c r="F48" s="102" t="s">
+        <v>126</v>
+      </c>
+      <c r="G48">
+        <f>SUM(G35:G47)</f>
+        <v>112325168</v>
+      </c>
+      <c r="H48">
+        <f t="shared" ref="H48:L48" si="2">SUM(H35:H47)</f>
+        <v>1245617</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="2"/>
+        <v>50143</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="2"/>
+        <v>506207</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="2"/>
+        <v>5771</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="2"/>
+        <v>13147443</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7">
+      <c r="G50">
+        <f>SUM(G48,J48:L48)</f>
+        <v>125984589</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7">
+      <c r="G51">
+        <f>I48+H48</f>
+        <v>1295760</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="TOC!A1" display="TOC" xr:uid="{4E4945F8-85AA-4C09-9CEC-835C946266DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FE28A6-DA79-4C04-860D-C3B0D186CA6A}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6739,6 +7115,373 @@
       <c r="L33" s="20"/>
       <c r="M33" s="20"/>
       <c r="P33" s="14"/>
+    </row>
+    <row r="35" spans="6:16">
+      <c r="G35">
+        <f>G7*G20</f>
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ref="H35:L35" si="0">H7*H20</f>
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="6:16">
+      <c r="G36">
+        <f t="shared" ref="G36:L49" si="1">G8*G21</f>
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="6:16">
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>214480</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="6:16">
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>306144</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="6:16">
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>830790</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>147489</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="6:16">
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>1215480</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>1238987</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>56000</v>
+      </c>
+      <c r="L40">
+        <f t="shared" si="1"/>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="41" spans="6:16">
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>3480960</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>1063188</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <f t="shared" si="1"/>
+        <v>22401</v>
+      </c>
+    </row>
+    <row r="42" spans="6:16">
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>2557224</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>920300</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="6:16">
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>1971762</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>1048572</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <f t="shared" si="1"/>
+        <v>94512</v>
+      </c>
+    </row>
+    <row r="44" spans="6:16">
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>1419314</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>798658</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <f t="shared" si="1"/>
+        <v>192605</v>
+      </c>
+    </row>
+    <row r="45" spans="6:16">
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>304750</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>318720</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <f t="shared" si="1"/>
+        <v>164406</v>
+      </c>
+    </row>
+    <row r="46" spans="6:16">
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>174660</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <f t="shared" si="1"/>
+        <v>44252</v>
+      </c>
+    </row>
+    <row r="47" spans="6:16">
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>13219</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>13801</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <f t="shared" si="1"/>
+        <v>45042</v>
+      </c>
+    </row>
+    <row r="48" spans="6:16">
+      <c r="F48" t="s">
+        <v>126</v>
+      </c>
+      <c r="G48">
+        <f>SUM(G35:G47)</f>
+        <v>11137369</v>
+      </c>
+      <c r="H48">
+        <f t="shared" ref="H48:L48" si="2">SUM(H35:H47)</f>
+        <v>37</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="2"/>
+        <v>6753640</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="2"/>
+        <v>203489</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="2"/>
+        <v>563731</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
add all four tiers in BART
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_BART_Demographics_20190630.xlsx
+++ b/inputs/data_raw/Data_BART_Demographics_20190630.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_BART\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8466A9B9-4A04-48FC-9D8F-52B217A420A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52657F80-05E8-4CEA-82DC-7B056FB439F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="723" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1500" windowWidth="29040" windowHeight="15840" tabRatio="723" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="actives_misc" sheetId="19" r:id="rId1"/>
@@ -4808,10 +4808,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F61A781-B9B1-4F2B-BAEA-4245EA889B53}">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6120,11 +6120,11 @@
         <v>112325168</v>
       </c>
       <c r="H48">
-        <f t="shared" ref="H48:L48" si="2">SUM(H35:H47)</f>
+        <f>SUM(H35:H47)</f>
         <v>1245617</v>
       </c>
       <c r="I48">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H48:L48" si="2">SUM(I35:I47)</f>
         <v>50143</v>
       </c>
       <c r="J48">
@@ -6150,6 +6150,12 @@
       <c r="G51">
         <f>I48+H48</f>
         <v>1295760</v>
+      </c>
+    </row>
+    <row r="52" spans="7:7">
+      <c r="G52">
+        <f>G51/113</f>
+        <v>11466.902654867257</v>
       </c>
     </row>
   </sheetData>
@@ -6164,10 +6170,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FE28A6-DA79-4C04-860D-C3B0D186CA6A}">
-  <dimension ref="A1:P48"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7481,6 +7487,18 @@
       <c r="L48">
         <f t="shared" si="2"/>
         <v>563731</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7">
+      <c r="G50">
+        <f>G48+J48+K48+L48</f>
+        <v>11904589</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7">
+      <c r="G51">
+        <f>SUM(H48:I48)</f>
+        <v>6753677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first working version for BART Misc
Issue in AL and NC of actives
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_BART_Demographics_20190630.xlsx
+++ b/inputs/data_raw/Data_BART_Demographics_20190630.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_BART\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52657F80-05E8-4CEA-82DC-7B056FB439F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F2E975-EE7B-4003-B40C-ABA8867C1B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1500" windowWidth="29040" windowHeight="15840" tabRatio="723" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1500" windowWidth="29040" windowHeight="15840" tabRatio="723" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="actives_misc" sheetId="19" r:id="rId1"/>
@@ -1733,13 +1733,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4810,7 +4810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F61A781-B9B1-4F2B-BAEA-4245EA889B53}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
@@ -5795,7 +5795,7 @@
     <row r="36" spans="6:16">
       <c r="F36" s="99"/>
       <c r="G36">
-        <f t="shared" ref="G36:L50" si="1">G8*G21</f>
+        <f t="shared" ref="G36:L47" si="1">G8*G21</f>
         <v>0</v>
       </c>
       <c r="H36">
@@ -6112,7 +6112,7 @@
       </c>
     </row>
     <row r="48" spans="6:16">
-      <c r="F48" s="102" t="s">
+      <c r="F48" s="100" t="s">
         <v>126</v>
       </c>
       <c r="G48">
@@ -6124,7 +6124,7 @@
         <v>1245617</v>
       </c>
       <c r="I48">
-        <f t="shared" ref="H48:L48" si="2">SUM(I35:I47)</f>
+        <f t="shared" ref="I48:L48" si="2">SUM(I35:I47)</f>
         <v>50143</v>
       </c>
       <c r="J48">
@@ -6172,7 +6172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FE28A6-DA79-4C04-860D-C3B0D186CA6A}">
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
@@ -7150,7 +7150,7 @@
     </row>
     <row r="36" spans="6:16">
       <c r="G36">
-        <f t="shared" ref="G36:L49" si="1">G8*G21</f>
+        <f t="shared" ref="G36:L47" si="1">G8*G21</f>
         <v>0</v>
       </c>
       <c r="H36">
@@ -7859,13 +7859,13 @@
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="B20" s="100" t="s">
+      <c r="B20" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="100"/>
-      <c r="D20" s="100"/>
-      <c r="E20" s="100"/>
-      <c r="F20" s="100"/>
+      <c r="C20" s="101"/>
+      <c r="D20" s="101"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="101"/>
       <c r="G20" s="62"/>
       <c r="H20" s="62"/>
       <c r="I20" s="62"/>
@@ -7873,12 +7873,12 @@
     <row r="21" spans="2:9">
       <c r="B21" s="63"/>
       <c r="C21" s="63"/>
-      <c r="D21" s="101" t="s">
+      <c r="D21" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="101"/>
-      <c r="F21" s="101"/>
-      <c r="G21" s="101"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
       <c r="H21" s="63"/>
       <c r="I21" s="63"/>
     </row>

</xml_diff>

<commit_message>
update analysis and html
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_BART_Demographics_20190630.xlsx
+++ b/inputs/data_raw/Data_BART_Demographics_20190630.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_BART\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C90DC29-A9DA-4E90-91BF-C885313742E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1868AD-D95C-45AD-8F28-933E04E27A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1500" windowWidth="29040" windowHeight="15840" tabRatio="723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="723" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="actives_misc" sheetId="19" r:id="rId1"/>
@@ -2511,15 +2511,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB403699-3710-4596-97B0-B33CB2C2CC4F}">
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z30" sqref="Z30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3271,6 +3272,272 @@
       </c>
       <c r="L28" s="13">
         <v>103937</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12">
+      <c r="G30">
+        <f>G9*G19</f>
+        <v>3435640</v>
+      </c>
+      <c r="H30">
+        <f t="shared" ref="H30:L30" si="0">H9*H19</f>
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12">
+      <c r="G31">
+        <f t="shared" ref="G31:L39" si="1">G10*G20</f>
+        <v>12546391</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>714924</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12">
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>22165348</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>5154510</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>771408</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>120844</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="7:12">
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>26981852</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>8418740</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>3750320</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>1243632</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>104515</v>
+      </c>
+      <c r="L33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="7:12">
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>25226850</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>7453176</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>6178362</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>2948633</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="1"/>
+        <v>1970623</v>
+      </c>
+      <c r="L34">
+        <f t="shared" si="1"/>
+        <v>689325</v>
+      </c>
+    </row>
+    <row r="35" spans="7:12">
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>19909749</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>6078800</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>6338574</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>6321024</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="1"/>
+        <v>6108291</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="1"/>
+        <v>3112256</v>
+      </c>
+    </row>
+    <row r="36" spans="7:12">
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>14669920</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>6882120</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>7003200</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>7383780</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>11199210</v>
+      </c>
+      <c r="L36">
+        <f t="shared" si="1"/>
+        <v>9515364</v>
+      </c>
+    </row>
+    <row r="37" spans="7:12">
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>14208051</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="1"/>
+        <v>5833292</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>7932844</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>7139181</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>11371920</v>
+      </c>
+      <c r="L37">
+        <f t="shared" si="1"/>
+        <v>12633543</v>
+      </c>
+    </row>
+    <row r="38" spans="7:12">
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>7276494</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="1"/>
+        <v>4289754</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>5284950</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>6356984</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>8721088</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="1"/>
+        <v>10538744</v>
+      </c>
+    </row>
+    <row r="39" spans="7:12">
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>1260112</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="1"/>
+        <v>1684160</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>3098884</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>3935280</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>5033650</v>
+      </c>
+      <c r="L39">
+        <f t="shared" si="1"/>
+        <v>5404724</v>
+      </c>
+    </row>
+    <row r="41" spans="7:12">
+      <c r="G41">
+        <f>SUM(G30:L39)</f>
+        <v>356401036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>